<commit_message>
EPBDS-9918 The first min/max condition in transposde SmartRules doesn't work
--HG--
branch : 5.23.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9179_SmartRuleWithInvalidNumberOfHConditions.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9179_SmartRuleWithInvalidNumberOfHConditions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkama\.openl\user-workspace\DEFAULT\Smart_hint (2) (2)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBF243A2-CE3A-4D40-B51C-E534B24AD044}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A12CB7-B83C-466B-9D8B-88E33A158628}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-30120" yWindow="6900" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>Result</t>
   </si>
@@ -51,10 +51,19 @@
     <t>=someMyRule5(2,3,4)</t>
   </si>
   <si>
-    <t>SmartLookup  MyObject2 someMyRule7(String var1, String b, Integer tst)</t>
-  </si>
-  <si>
     <t>Var1</t>
+  </si>
+  <si>
+    <t>SmartLookup  MyObject2 someMyRule7(String var1, String b)</t>
+  </si>
+  <si>
+    <t>4141</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
@@ -90,15 +99,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,188 +482,240 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C6:I86"/>
+  <dimension ref="B6:I87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:L31"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="I91" sqref="I91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="24.54296875" customWidth="1"/>
-    <col min="4" max="4" width="17.1796875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="28.81640625" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="39.453125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="39.42578125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-    </row>
-    <row r="21" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-    </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D40" t="s">
+    <row r="6" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="21" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D40" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="H40" t="s">
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D41" t="s">
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D41" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H41" t="s">
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D42" t="s">
+    <row r="42" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D42" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E42" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H42" t="s">
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="45" spans="4:9" x14ac:dyDescent="0.35">
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="1"/>
-      <c r="H45" s="1"/>
-      <c r="I45" s="1"/>
-    </row>
-    <row r="61" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C61" s="3"/>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-    </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-    </row>
-    <row r="67" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-    </row>
-    <row r="68" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-    </row>
-    <row r="69" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="D69" s="1"/>
-    </row>
-    <row r="74" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="C74" s="3"/>
-      <c r="D74" s="3"/>
-      <c r="E74" s="3"/>
-      <c r="F74" s="1"/>
-    </row>
-    <row r="76" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="D76" s="2"/>
-      <c r="F76" s="2"/>
-    </row>
-    <row r="77" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="D77" s="2"/>
-      <c r="F77" s="2"/>
-    </row>
-    <row r="78" spans="3:6" x14ac:dyDescent="0.35">
-      <c r="D78" s="2"/>
-      <c r="F78" s="2"/>
-    </row>
-    <row r="81" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C81" s="3" t="s">
+    <row r="45" spans="4:9" x14ac:dyDescent="0.25">
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2"/>
+    </row>
+    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C62" s="4"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="4"/>
+    </row>
+    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+      <c r="E67" s="2"/>
+      <c r="F67" s="2"/>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C68" s="4"/>
+      <c r="D68" s="5"/>
+      <c r="E68" s="5"/>
+      <c r="F68" s="4"/>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C69" s="4"/>
+      <c r="D69" s="5"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+    </row>
+    <row r="74" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C74" s="2"/>
+      <c r="D74" s="2"/>
+      <c r="E74" s="2"/>
+      <c r="F74" s="5"/>
+    </row>
+    <row r="76" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C76" s="4"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="6"/>
+    </row>
+    <row r="77" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C77" s="4"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="6"/>
+    </row>
+    <row r="78" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C78" s="4"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="6"/>
+    </row>
+    <row r="81" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B81" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" s="2"/>
+      <c r="D81" s="2"/>
+      <c r="E81" s="3"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="4"/>
+    </row>
+    <row r="82" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B82" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D81" s="3"/>
-      <c r="E81" s="3"/>
-    </row>
-    <row r="82" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C82" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D82" s="3" t="s">
+      <c r="C82" s="2"/>
+      <c r="D82" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E82" s="3"/>
-    </row>
-    <row r="83" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C83" s="3"/>
-      <c r="D83" s="1">
+      <c r="F82" s="7"/>
+      <c r="G82" s="4"/>
+    </row>
+    <row r="83" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="5">
         <v>2</v>
       </c>
-      <c r="E83" s="1">
+      <c r="E83" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="84" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C84" s="3"/>
-      <c r="D84">
+      <c r="F83" s="4"/>
+      <c r="G83" s="4"/>
+    </row>
+    <row r="84" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B84" s="2"/>
+      <c r="C84" s="2"/>
+      <c r="D84" s="4">
         <v>1</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E84" s="6">
         <v>12</v>
       </c>
-      <c r="F84" s="2"/>
-      <c r="G84" s="2"/>
-    </row>
-    <row r="85" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="D85" s="2" t="s">
+      <c r="F84" s="4"/>
+      <c r="G84" s="6"/>
+    </row>
+    <row r="85" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E85">
+      <c r="E85" s="4">
         <v>3</v>
       </c>
-    </row>
-    <row r="86" spans="3:7" x14ac:dyDescent="0.35">
-      <c r="C86">
+      <c r="F85" s="4"/>
+      <c r="G85" s="4"/>
+    </row>
+    <row r="86" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B86" s="4"/>
+      <c r="C86" s="4">
         <v>3131</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="4">
         <v>0</v>
       </c>
-      <c r="E86" s="2" t="s">
+      <c r="E86" s="6" t="s">
         <v>8</v>
       </c>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
+    </row>
+    <row r="87" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B87" s="4"/>
+      <c r="C87" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E87" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="F87" s="4"/>
+      <c r="G87" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C67:F67"/>
+    <mergeCell ref="B82:C84"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="B81:E81"/>
     <mergeCell ref="D6:I6"/>
     <mergeCell ref="D21:I21"/>
     <mergeCell ref="D45:F45"/>
     <mergeCell ref="D62:E62"/>
     <mergeCell ref="C61:F61"/>
-    <mergeCell ref="C82:C84"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C81:E81"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="C67:F67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -659,7 +727,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -671,7 +739,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>